<commit_message>
Enhanced visualization readability - increased font sizes, larger graphs, and improved styling
- Increased base font size from 12-14 to 16-18 for better readability
- Enlarged graph dimensions: individual plots (12x10  16x12), comprehensive plots (24x16  28x20)
- Enhanced line thickness (1.5  3.0) and added markers for better data visibility
- Improved legends with shadows, fancy boxes, and better positioning
- Added professional styling: bold fonts, consistent colors, enhanced grids
- Updated all comparison plots (15 total) with new readability standards
- Upgraded visualization exports to 300 DPI with bbox_inches='tight' for presentations
- Maintained consistent color scheme: R1=Green, R2=Red, R3=Blue across all visualizations
</commit_message>
<xml_diff>
--- a/Reaction-1.xlsx
+++ b/Reaction-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABHISHEK KUMAWAT\Downloads\current Ps\q1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding Related Items\Web Dev\python\plots for dr reddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{365D0792-8244-45D9-84BE-64B51EDC9563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D5A4D7-FFAF-4ADB-A0A6-4BD844E2A7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" r:id="rId1"/>
@@ -488,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -4319,7 +4319,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N166"/>
   <sheetViews>
-    <sheetView zoomScale="79" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4327,7 +4329,7 @@
     <col min="8" max="8" width="13.88671875" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="14.5546875" customWidth="1"/>
-    <col min="11" max="11" width="17.109375" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" customWidth="1"/>
     <col min="12" max="12" width="15.77734375" customWidth="1"/>
     <col min="13" max="13" width="21.44140625" customWidth="1"/>
     <col min="14" max="14" width="25.109375" customWidth="1"/>

</xml_diff>